<commit_message>
nettoyge des vieux fichiers, et ajout de la transposition au DF d'impact poste
</commit_message>
<xml_diff>
--- a/Excel/TI/Mon_TI_2024_02_11.xlsx
+++ b/Excel/TI/Mon_TI_2024_02_11.xlsx
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>30.6</v>
+        <v>35.2</v>
       </c>
       <c r="F2" t="n">
         <v>26.3</v>
@@ -657,29 +657,29 @@
         <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L2" t="n">
         <v>2</v>
       </c>
       <c r="M2" t="n">
+        <v>30</v>
+      </c>
+      <c r="N2" t="n">
         <v>44</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>32</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>30</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>40</v>
       </c>
-      <c r="Q2" t="n">
-        <v>7</v>
-      </c>
       <c r="R2" t="inlineStr">
         <is>
           <t>vs</t>
@@ -692,11 +692,11 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="U2" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="V2" t="inlineStr">
         <is>
@@ -760,14 +760,18 @@
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AI2" t="n">
-        <v>-1.1</v>
-      </c>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="inlineStr"/>
+        <v>1.1</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>-7.4</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -787,22 +791,22 @@
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>26.8</v>
+        <v>30.6</v>
       </c>
       <c r="F3" t="n">
-        <v>33.1</v>
+        <v>32.5</v>
       </c>
       <c r="G3" t="n">
-        <v>30.7</v>
+        <v>30.6</v>
       </c>
       <c r="H3" t="n">
         <v>12</v>
       </c>
       <c r="I3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K3" t="n">
         <v>2</v>
@@ -813,20 +817,20 @@
       <c r="M3" t="n">
         <v>28</v>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O3" t="n">
+      <c r="N3" t="n">
+        <v>28</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
         <v>14</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>41</v>
       </c>
-      <c r="Q3" t="n">
-        <v>42</v>
-      </c>
       <c r="R3" t="inlineStr">
         <is>
           <t>@</t>
@@ -843,17 +847,15 @@
         </is>
       </c>
       <c r="U3" t="n">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="W3" t="n">
+        <v>31</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
@@ -907,11 +909,11 @@
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AI3" t="n">
-        <v>1.6</v>
+        <v>-1.8</v>
       </c>
       <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
@@ -934,13 +936,13 @@
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>26.4</v>
+        <v>30.2</v>
       </c>
       <c r="F4" t="n">
-        <v>31.1</v>
+        <v>30.7</v>
       </c>
       <c r="G4" t="n">
-        <v>35.6</v>
+        <v>35.4</v>
       </c>
       <c r="H4" t="n">
         <v>13</v>
@@ -958,20 +960,20 @@
         <v>4</v>
       </c>
       <c r="M4" t="n">
+        <v>28</v>
+      </c>
+      <c r="N4" t="n">
         <v>15</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>17</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>60</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>31</v>
       </c>
-      <c r="Q4" t="n">
-        <v>9</v>
-      </c>
       <c r="R4" t="inlineStr">
         <is>
           <t>@</t>
@@ -988,7 +990,7 @@
         </is>
       </c>
       <c r="U4" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="V4" t="inlineStr">
         <is>
@@ -1052,11 +1054,11 @@
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AI4" t="n">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
       <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>

</xml_diff>